<commit_message>
added most recent and least recent dates
</commit_message>
<xml_diff>
--- a/Sum.xlsx
+++ b/Sum.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="70">
   <si>
     <t>DeliveryID</t>
   </si>
@@ -212,6 +212,18 @@
   </si>
   <si>
     <t>Missed</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>Last Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jul 21 2022 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jul  1 2022 </t>
   </si>
 </sst>
 </file>
@@ -590,7 +602,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D254"/>
+  <dimension ref="A1:G254"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -599,10 +611,12 @@
     <col min="1" max="1" width="25.7109375" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
     <col min="3" max="3" width="25.7109375" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -615,8 +629,14 @@
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" s="2" customFormat="1">
+      <c r="F1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="2" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -629,8 +649,14 @@
       <c r="D2" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" s="3" customFormat="1">
+      <c r="F2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="3" customFormat="1">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
@@ -640,7 +666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="2" customFormat="1">
+    <row r="4" spans="1:7" s="2" customFormat="1">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>7</v>
@@ -652,7 +678,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="3" customFormat="1">
+    <row r="5" spans="1:7" s="3" customFormat="1">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
@@ -662,7 +688,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="2" customFormat="1">
+    <row r="6" spans="1:7" s="2" customFormat="1">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>8</v>
@@ -674,7 +700,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="3" customFormat="1">
+    <row r="7" spans="1:7" s="3" customFormat="1">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
@@ -684,7 +710,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="2" customFormat="1">
+    <row r="8" spans="1:7" s="2" customFormat="1">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
@@ -694,7 +720,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="3" customFormat="1">
+    <row r="9" spans="1:7" s="3" customFormat="1">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>9</v>
@@ -706,7 +732,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="2" customFormat="1">
+    <row r="10" spans="1:7" s="2" customFormat="1">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
@@ -716,7 +742,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="3" customFormat="1">
+    <row r="11" spans="1:7" s="3" customFormat="1">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
@@ -726,7 +752,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="2" customFormat="1">
+    <row r="12" spans="1:7" s="2" customFormat="1">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
         <v>10</v>
@@ -738,7 +764,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="3" customFormat="1">
+    <row r="13" spans="1:7" s="3" customFormat="1">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
@@ -748,7 +774,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="2" customFormat="1">
+    <row r="14" spans="1:7" s="2" customFormat="1">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
@@ -758,7 +784,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="3" customFormat="1">
+    <row r="15" spans="1:7" s="3" customFormat="1">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
@@ -768,7 +794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="2" customFormat="1">
+    <row r="16" spans="1:7" s="2" customFormat="1">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">

</xml_diff>

<commit_message>
Took out coloration, aligned totals to left
</commit_message>
<xml_diff>
--- a/Sum.xlsx
+++ b/Sum.xlsx
@@ -218,7 +218,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -234,32 +234,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF0CA86"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF9AD7A4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -289,13 +270,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -599,7 +581,7 @@
     <col min="1" max="1" width="25.7109375" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
     <col min="3" max="3" width="25.7109375" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
     <col min="6" max="6" width="20.7109375" customWidth="1"/>
     <col min="7" max="7" width="20.7109375" customWidth="1"/>
   </cols>
@@ -614,8 +596,8 @@
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
+      <c r="D1" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="F1" t="s">
         <v>62</v>
@@ -637,9 +619,6 @@
       <c r="D2" s="2">
         <v>1</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="F2" s="2" t="s">
         <v>63</v>
       </c>
@@ -647,7 +626,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="3" customFormat="1">
+    <row r="3" spans="1:7" s="2" customFormat="1">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>7</v>
@@ -655,7 +634,7 @@
       <c r="C3" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>6</v>
       </c>
     </row>
@@ -671,7 +650,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="3" customFormat="1">
+    <row r="5" spans="1:7" s="2" customFormat="1">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>9</v>
@@ -679,7 +658,7 @@
       <c r="C5" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>14</v>
       </c>
     </row>
@@ -693,7 +672,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="3" customFormat="1">
+    <row r="7" spans="1:7" s="2" customFormat="1">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>10</v>
@@ -701,7 +680,7 @@
       <c r="C7" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>4</v>
       </c>
     </row>
@@ -717,7 +696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="3" customFormat="1">
+    <row r="9" spans="1:7" s="2" customFormat="1">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>12</v>
@@ -725,7 +704,7 @@
       <c r="C9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>2</v>
       </c>
     </row>
@@ -741,13 +720,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="3" customFormat="1">
+    <row r="11" spans="1:7" s="2" customFormat="1">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <v>1</v>
       </c>
     </row>
@@ -761,7 +740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="3" customFormat="1">
+    <row r="13" spans="1:7" s="2" customFormat="1">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
         <v>14</v>
@@ -769,7 +748,7 @@
       <c r="C13" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="2">
         <v>2</v>
       </c>
     </row>
@@ -785,13 +764,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="3" customFormat="1">
+    <row r="15" spans="1:7" s="2" customFormat="1">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="2">
         <v>6</v>
       </c>
     </row>
@@ -807,7 +786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="3" customFormat="1">
+    <row r="17" spans="1:4" s="2" customFormat="1">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
         <v>17</v>
@@ -815,7 +794,7 @@
       <c r="C17" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="2">
         <v>2</v>
       </c>
     </row>
@@ -831,13 +810,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="3" customFormat="1">
+    <row r="19" spans="1:4" s="2" customFormat="1">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="2">
         <v>1</v>
       </c>
     </row>
@@ -853,13 +832,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="3" customFormat="1">
+    <row r="21" spans="1:4" s="2" customFormat="1">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="2">
         <v>1</v>
       </c>
     </row>
@@ -875,13 +854,13 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="3" customFormat="1">
+    <row r="23" spans="1:4" s="2" customFormat="1">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="2">
         <v>4</v>
       </c>
     </row>
@@ -897,7 +876,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:4" s="3" customFormat="1">
+    <row r="25" spans="1:4" s="2" customFormat="1">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
         <v>22</v>
@@ -905,7 +884,7 @@
       <c r="C25" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="2">
         <v>1</v>
       </c>
     </row>
@@ -921,7 +900,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:4" s="3" customFormat="1">
+    <row r="27" spans="1:4" s="2" customFormat="1">
       <c r="A27" s="1"/>
       <c r="B27" s="1" t="s">
         <v>24</v>
@@ -929,7 +908,7 @@
       <c r="C27" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27" s="2">
         <v>1</v>
       </c>
     </row>
@@ -943,7 +922,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:4" s="3" customFormat="1">
+    <row r="29" spans="1:4" s="2" customFormat="1">
       <c r="A29" s="1"/>
       <c r="B29" s="1" t="s">
         <v>25</v>
@@ -951,7 +930,7 @@
       <c r="C29" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D29" s="2">
         <v>1</v>
       </c>
     </row>
@@ -965,7 +944,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:4" s="3" customFormat="1">
+    <row r="31" spans="1:4" s="2" customFormat="1">
       <c r="A31" s="1"/>
       <c r="B31" s="1" t="s">
         <v>26</v>
@@ -973,7 +952,7 @@
       <c r="C31" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D31" s="3">
+      <c r="D31" s="2">
         <v>10</v>
       </c>
     </row>
@@ -989,13 +968,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:4" s="3" customFormat="1">
+    <row r="33" spans="1:4" s="2" customFormat="1">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D33" s="3">
+      <c r="D33" s="2">
         <v>7</v>
       </c>
     </row>
@@ -1011,7 +990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:4" s="3" customFormat="1">
+    <row r="35" spans="1:4" s="2" customFormat="1">
       <c r="A35" s="1"/>
       <c r="B35" s="1" t="s">
         <v>29</v>
@@ -1019,7 +998,7 @@
       <c r="C35" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D35" s="3">
+      <c r="D35" s="2">
         <v>6</v>
       </c>
     </row>
@@ -1035,7 +1014,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="37" spans="1:4" s="3" customFormat="1">
+    <row r="37" spans="1:4" s="2" customFormat="1">
       <c r="A37" s="1"/>
       <c r="B37" s="1" t="s">
         <v>31</v>
@@ -1043,7 +1022,7 @@
       <c r="C37" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D37" s="3">
+      <c r="D37" s="2">
         <v>1</v>
       </c>
     </row>
@@ -1057,13 +1036,13 @@
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="1:4" s="3" customFormat="1">
+    <row r="39" spans="1:4" s="2" customFormat="1">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D39" s="3">
+      <c r="D39" s="2">
         <v>2</v>
       </c>
     </row>
@@ -1079,13 +1058,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:4" s="3" customFormat="1">
+    <row r="41" spans="1:4" s="2" customFormat="1">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D41" s="3">
+      <c r="D41" s="2">
         <v>1</v>
       </c>
     </row>
@@ -1099,7 +1078,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:4" s="3" customFormat="1">
+    <row r="43" spans="1:4" s="2" customFormat="1">
       <c r="A43" s="1"/>
       <c r="B43" s="1" t="s">
         <v>33</v>
@@ -1107,7 +1086,7 @@
       <c r="C43" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D43" s="3">
+      <c r="D43" s="2">
         <v>53</v>
       </c>
     </row>
@@ -1121,7 +1100,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:4" s="3" customFormat="1">
+    <row r="45" spans="1:4" s="2" customFormat="1">
       <c r="A45" s="1"/>
       <c r="B45" s="1" t="s">
         <v>34</v>
@@ -1129,7 +1108,7 @@
       <c r="C45" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D45" s="3">
+      <c r="D45" s="2">
         <v>1</v>
       </c>
     </row>
@@ -1145,13 +1124,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:4" s="3" customFormat="1">
+    <row r="47" spans="1:4" s="2" customFormat="1">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D47" s="3">
+      <c r="D47" s="2">
         <v>23</v>
       </c>
     </row>
@@ -1165,7 +1144,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:4" s="3" customFormat="1">
+    <row r="49" spans="1:4" s="2" customFormat="1">
       <c r="A49" s="1"/>
       <c r="B49" s="1" t="s">
         <v>36</v>
@@ -1173,7 +1152,7 @@
       <c r="C49" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D49" s="3">
+      <c r="D49" s="2">
         <v>1</v>
       </c>
     </row>
@@ -1189,7 +1168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:4" s="3" customFormat="1">
+    <row r="51" spans="1:4" s="2" customFormat="1">
       <c r="A51" s="1"/>
       <c r="B51" s="1" t="s">
         <v>38</v>
@@ -1197,7 +1176,7 @@
       <c r="C51" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D51" s="3">
+      <c r="D51" s="2">
         <v>2</v>
       </c>
     </row>
@@ -1213,7 +1192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:4" s="3" customFormat="1">
+    <row r="53" spans="1:4" s="2" customFormat="1">
       <c r="A53" s="1"/>
       <c r="B53" s="1" t="s">
         <v>40</v>
@@ -1221,7 +1200,7 @@
       <c r="C53" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D53" s="3">
+      <c r="D53" s="2">
         <v>3</v>
       </c>
     </row>
@@ -1235,7 +1214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:4" s="3" customFormat="1">
+    <row r="55" spans="1:4" s="2" customFormat="1">
       <c r="A55" s="1"/>
       <c r="B55" s="1" t="s">
         <v>41</v>
@@ -1243,7 +1222,7 @@
       <c r="C55" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D55" s="3">
+      <c r="D55" s="2">
         <v>3</v>
       </c>
     </row>
@@ -1257,7 +1236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:4" s="3" customFormat="1">
+    <row r="57" spans="1:4" s="2" customFormat="1">
       <c r="A57" s="1"/>
       <c r="B57" s="1" t="s">
         <v>42</v>
@@ -1265,7 +1244,7 @@
       <c r="C57" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D57" s="3">
+      <c r="D57" s="2">
         <v>3</v>
       </c>
     </row>
@@ -1281,7 +1260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:4" s="3" customFormat="1">
+    <row r="59" spans="1:4" s="2" customFormat="1">
       <c r="A59" s="1"/>
       <c r="B59" s="1" t="s">
         <v>44</v>
@@ -1289,7 +1268,7 @@
       <c r="C59" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D59" s="3">
+      <c r="D59" s="2">
         <v>3</v>
       </c>
     </row>
@@ -1305,7 +1284,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:4" s="3" customFormat="1">
+    <row r="61" spans="1:4" s="2" customFormat="1">
       <c r="A61" s="1"/>
       <c r="B61" s="1" t="s">
         <v>46</v>
@@ -1313,7 +1292,7 @@
       <c r="C61" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D61" s="3">
+      <c r="D61" s="2">
         <v>1</v>
       </c>
     </row>
@@ -1329,7 +1308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:4" s="3" customFormat="1">
+    <row r="63" spans="1:4" s="2" customFormat="1">
       <c r="A63" s="1" t="s">
         <v>5</v>
       </c>
@@ -1339,7 +1318,7 @@
       <c r="C63" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D63" s="3">
+      <c r="D63" s="2">
         <v>6</v>
       </c>
     </row>
@@ -1353,7 +1332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:4" s="3" customFormat="1">
+    <row r="65" spans="1:4" s="2" customFormat="1">
       <c r="A65" s="1"/>
       <c r="B65" s="1" t="s">
         <v>48</v>
@@ -1361,7 +1340,7 @@
       <c r="C65" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D65" s="3">
+      <c r="D65" s="2">
         <v>1</v>
       </c>
     </row>
@@ -1377,13 +1356,13 @@
         <v>32</v>
       </c>
     </row>
-    <row r="67" spans="1:4" s="3" customFormat="1">
+    <row r="67" spans="1:4" s="2" customFormat="1">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D67" s="3">
+      <c r="D67" s="2">
         <v>2</v>
       </c>
     </row>
@@ -1399,13 +1378,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="69" spans="1:4" s="3" customFormat="1">
+    <row r="69" spans="1:4" s="2" customFormat="1">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D69" s="3">
+      <c r="D69" s="2">
         <v>2</v>
       </c>
     </row>
@@ -1421,7 +1400,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:4" s="3" customFormat="1">
+    <row r="71" spans="1:4" s="2" customFormat="1">
       <c r="A71" s="1"/>
       <c r="B71" s="1" t="s">
         <v>49</v>
@@ -1429,7 +1408,7 @@
       <c r="C71" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D71" s="3">
+      <c r="D71" s="2">
         <v>3</v>
       </c>
     </row>
@@ -1445,7 +1424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:4" s="3" customFormat="1">
+    <row r="73" spans="1:4" s="2" customFormat="1">
       <c r="A73" s="1"/>
       <c r="B73" s="1" t="s">
         <v>12</v>
@@ -1453,7 +1432,7 @@
       <c r="C73" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D73" s="3">
+      <c r="D73" s="2">
         <v>10</v>
       </c>
     </row>
@@ -1469,13 +1448,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="75" spans="1:4" s="3" customFormat="1">
+    <row r="75" spans="1:4" s="2" customFormat="1">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D75" s="3">
+      <c r="D75" s="2">
         <v>3</v>
       </c>
     </row>
@@ -1491,13 +1470,13 @@
         <v>22</v>
       </c>
     </row>
-    <row r="77" spans="1:4" s="3" customFormat="1">
+    <row r="77" spans="1:4" s="2" customFormat="1">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D77" s="3">
+      <c r="D77" s="2">
         <v>5</v>
       </c>
     </row>
@@ -1513,7 +1492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:4" s="3" customFormat="1">
+    <row r="79" spans="1:4" s="2" customFormat="1">
       <c r="A79" s="1"/>
       <c r="B79" s="1" t="s">
         <v>17</v>
@@ -1521,7 +1500,7 @@
       <c r="C79" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D79" s="3">
+      <c r="D79" s="2">
         <v>7</v>
       </c>
     </row>
@@ -1537,7 +1516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:4" s="3" customFormat="1">
+    <row r="81" spans="1:4" s="2" customFormat="1">
       <c r="A81" s="1"/>
       <c r="B81" s="1" t="s">
         <v>52</v>
@@ -1545,7 +1524,7 @@
       <c r="C81" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D81" s="3">
+      <c r="D81" s="2">
         <v>1</v>
       </c>
     </row>
@@ -1559,7 +1538,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:4" s="3" customFormat="1">
+    <row r="83" spans="1:4" s="2" customFormat="1">
       <c r="A83" s="1"/>
       <c r="B83" s="1" t="s">
         <v>18</v>
@@ -1567,7 +1546,7 @@
       <c r="C83" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D83" s="3">
+      <c r="D83" s="2">
         <v>7</v>
       </c>
     </row>
@@ -1581,7 +1560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:4" s="3" customFormat="1">
+    <row r="85" spans="1:4" s="2" customFormat="1">
       <c r="A85" s="1"/>
       <c r="B85" s="1" t="s">
         <v>19</v>
@@ -1589,7 +1568,7 @@
       <c r="C85" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D85" s="3">
+      <c r="D85" s="2">
         <v>7</v>
       </c>
     </row>
@@ -1605,13 +1584,13 @@
         <v>26</v>
       </c>
     </row>
-    <row r="87" spans="1:4" s="3" customFormat="1">
+    <row r="87" spans="1:4" s="2" customFormat="1">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D87" s="3">
+      <c r="D87" s="2">
         <v>3</v>
       </c>
     </row>
@@ -1627,7 +1606,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:4" s="3" customFormat="1">
+    <row r="89" spans="1:4" s="2" customFormat="1">
       <c r="A89" s="1"/>
       <c r="B89" s="1" t="s">
         <v>24</v>
@@ -1635,7 +1614,7 @@
       <c r="C89" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D89" s="3">
+      <c r="D89" s="2">
         <v>11</v>
       </c>
     </row>
@@ -1649,7 +1628,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="1:4" s="3" customFormat="1">
+    <row r="91" spans="1:4" s="2" customFormat="1">
       <c r="A91" s="1"/>
       <c r="B91" s="1" t="s">
         <v>53</v>
@@ -1657,7 +1636,7 @@
       <c r="C91" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D91" s="3">
+      <c r="D91" s="2">
         <v>4</v>
       </c>
     </row>
@@ -1673,13 +1652,13 @@
         <v>11</v>
       </c>
     </row>
-    <row r="93" spans="1:4" s="3" customFormat="1">
+    <row r="93" spans="1:4" s="2" customFormat="1">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D93" s="3">
+      <c r="D93" s="2">
         <v>1</v>
       </c>
     </row>
@@ -1695,13 +1674,13 @@
         <v>22</v>
       </c>
     </row>
-    <row r="95" spans="1:4" s="3" customFormat="1">
+    <row r="95" spans="1:4" s="2" customFormat="1">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D95" s="3">
+      <c r="D95" s="2">
         <v>3</v>
       </c>
     </row>
@@ -1717,7 +1696,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="97" spans="1:4" s="3" customFormat="1">
+    <row r="97" spans="1:4" s="2" customFormat="1">
       <c r="A97" s="1"/>
       <c r="B97" s="1" t="s">
         <v>29</v>
@@ -1725,7 +1704,7 @@
       <c r="C97" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D97" s="3">
+      <c r="D97" s="2">
         <v>10</v>
       </c>
     </row>
@@ -1741,7 +1720,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="99" spans="1:4" s="3" customFormat="1">
+    <row r="99" spans="1:4" s="2" customFormat="1">
       <c r="A99" s="1"/>
       <c r="B99" s="1" t="s">
         <v>31</v>
@@ -1749,7 +1728,7 @@
       <c r="C99" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D99" s="3">
+      <c r="D99" s="2">
         <v>42</v>
       </c>
     </row>
@@ -1765,7 +1744,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="101" spans="1:4" s="3" customFormat="1">
+    <row r="101" spans="1:4" s="2" customFormat="1">
       <c r="A101" s="1"/>
       <c r="B101" s="1" t="s">
         <v>33</v>
@@ -1773,7 +1752,7 @@
       <c r="C101" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D101" s="3">
+      <c r="D101" s="2">
         <v>41</v>
       </c>
     </row>
@@ -1787,7 +1766,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:4" s="3" customFormat="1">
+    <row r="103" spans="1:4" s="2" customFormat="1">
       <c r="A103" s="1"/>
       <c r="B103" s="1" t="s">
         <v>54</v>
@@ -1795,7 +1774,7 @@
       <c r="C103" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D103" s="3">
+      <c r="D103" s="2">
         <v>6</v>
       </c>
     </row>
@@ -1811,13 +1790,13 @@
         <v>73</v>
       </c>
     </row>
-    <row r="105" spans="1:4" s="3" customFormat="1">
+    <row r="105" spans="1:4" s="2" customFormat="1">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D105" s="3">
+      <c r="D105" s="2">
         <v>1</v>
       </c>
     </row>
@@ -1831,7 +1810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:4" s="3" customFormat="1">
+    <row r="107" spans="1:4" s="2" customFormat="1">
       <c r="A107" s="1"/>
       <c r="B107" s="1" t="s">
         <v>36</v>
@@ -1839,7 +1818,7 @@
       <c r="C107" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D107" s="3">
+      <c r="D107" s="2">
         <v>3</v>
       </c>
     </row>
@@ -1855,7 +1834,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="109" spans="1:4" s="3" customFormat="1">
+    <row r="109" spans="1:4" s="2" customFormat="1">
       <c r="A109" s="1"/>
       <c r="B109" s="1" t="s">
         <v>39</v>
@@ -1863,7 +1842,7 @@
       <c r="C109" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D109" s="3">
+      <c r="D109" s="2">
         <v>6</v>
       </c>
     </row>
@@ -1877,7 +1856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:4" s="3" customFormat="1">
+    <row r="111" spans="1:4" s="2" customFormat="1">
       <c r="A111" s="1"/>
       <c r="B111" s="1" t="s">
         <v>41</v>
@@ -1885,7 +1864,7 @@
       <c r="C111" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D111" s="3">
+      <c r="D111" s="2">
         <v>2</v>
       </c>
     </row>
@@ -1901,7 +1880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:4" s="3" customFormat="1">
+    <row r="113" spans="1:4" s="2" customFormat="1">
       <c r="A113" s="1"/>
       <c r="B113" s="1" t="s">
         <v>55</v>
@@ -1909,7 +1888,7 @@
       <c r="C113" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D113" s="3">
+      <c r="D113" s="2">
         <v>2</v>
       </c>
     </row>
@@ -1925,13 +1904,13 @@
         <v>16</v>
       </c>
     </row>
-    <row r="115" spans="1:4" s="3" customFormat="1">
+    <row r="115" spans="1:4" s="2" customFormat="1">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D115" s="3">
+      <c r="D115" s="2">
         <v>1</v>
       </c>
     </row>
@@ -1947,7 +1926,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="117" spans="1:4" s="3" customFormat="1">
+    <row r="117" spans="1:4" s="2" customFormat="1">
       <c r="A117" s="1"/>
       <c r="B117" s="1" t="s">
         <v>47</v>
@@ -1955,7 +1934,7 @@
       <c r="C117" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D117" s="3">
+      <c r="D117" s="2">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Standard directory is downloads
</commit_message>
<xml_diff>
--- a/Sum.xlsx
+++ b/Sum.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="65">
   <si>
     <t>DeliveryID</t>
   </si>
@@ -209,9 +209,6 @@
   </si>
   <si>
     <t xml:space="preserve">Jul 11 2022 </t>
-  </si>
-  <si>
-    <t>Totals</t>
   </si>
 </sst>
 </file>
@@ -596,8 +593,8 @@
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>65</v>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="F1" t="s">
         <v>62</v>
@@ -1938,13 +1935,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="118" spans="1:4">
+    <row r="118" spans="1:4" s="2" customFormat="1">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D118">
+      <c r="D118" s="2">
         <v>2</v>
       </c>
     </row>

</xml_diff>